<commit_message>
fix potsdam pop data, test mode figure updates
</commit_message>
<xml_diff>
--- a/outputs/density_geounits/summary_stats_Potsdam.xlsx
+++ b/outputs/density_geounits/summary_stats_Potsdam.xlsx
@@ -575,7 +575,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>178253</v>
+        <v>178185</v>
       </c>
     </row>
     <row r="4">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>946.4440019519508</v>
+        <v>946.0829522521828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>